<commit_message>
updates for week 3 and misc
</commit_message>
<xml_diff>
--- a/teaching/expdes/master-plan.xlsx
+++ b/teaching/expdes/master-plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38600" yWindow="5000" windowWidth="26260" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="43340" yWindow="1020" windowWidth="24320" windowHeight="20320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -278,6 +278,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="9">
@@ -350,7 +355,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -362,10 +367,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -661,7 +667,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,7 +767,7 @@
         <f>B4+7</f>
         <v>30</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1"/>
@@ -793,7 +799,7 @@
       <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="8"/>
@@ -808,7 +814,7 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2">
-        <f>B7+7</f>
+        <f t="shared" ref="B9:B14" si="0">B7+7</f>
         <v>8</v>
       </c>
       <c r="C9" s="8"/>
@@ -824,7 +830,7 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2">
-        <f>B8+7</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -842,7 +848,7 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2">
-        <f>B9+7</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C11" s="8"/>
@@ -858,14 +864,14 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2">
-        <f>B10+7</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>57</v>
       </c>
       <c r="F12" s="2"/>
@@ -876,7 +882,7 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2">
-        <f>B11+7</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C13" s="8"/>
@@ -892,14 +898,14 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2">
-        <f>B12+7</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="2"/>
@@ -987,7 +993,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="9"/>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>59</v>
       </c>
       <c r="F20" s="5"/>
@@ -1083,7 +1089,7 @@
         <v>20</v>
       </c>
       <c r="D26" s="10"/>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>60</v>
       </c>
       <c r="F26" s="6"/>

</xml_diff>

<commit_message>
adds for lecture 4
</commit_message>
<xml_diff>
--- a/teaching/expdes/master-plan.xlsx
+++ b/teaching/expdes/master-plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43340" yWindow="1020" windowWidth="24320" windowHeight="20320" tabRatio="500"/>
+    <workbookView xWindow="34860" yWindow="460" windowWidth="24320" windowHeight="20320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,55 +191,48 @@
     <t>WS 3-4</t>
   </si>
   <si>
+    <t>WS 6-9</t>
+  </si>
+  <si>
+    <t>WS 10-13</t>
+  </si>
+  <si>
+    <t>WS 14-16</t>
+  </si>
+  <si>
+    <t>WS 17-18</t>
+  </si>
+  <si>
+    <t>ME 12</t>
+  </si>
+  <si>
+    <t>FELS 25</t>
+  </si>
+  <si>
+    <t>HW10</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">WS 5 </t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
       <t>ME 2</t>
     </r>
-  </si>
-  <si>
-    <t>WS 6-9</t>
-  </si>
-  <si>
-    <t>WS 10-13</t>
-  </si>
-  <si>
-    <t>WS 14-16</t>
-  </si>
-  <si>
-    <t>WS 17-18</t>
-  </si>
-  <si>
-    <t>ME 12</t>
-  </si>
-  <si>
-    <t>FELS 25</t>
-  </si>
-  <si>
-    <t>HW10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -269,20 +262,15 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF808080"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="9">
@@ -346,16 +334,16 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -364,14 +352,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -667,7 +659,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,12 +759,12 @@
         <f>B4+7</f>
         <v>30</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>54</v>
+      <c r="E6" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -785,7 +777,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="8"/>
@@ -799,12 +791,12 @@
       <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="8" t="s">
-        <v>55</v>
+      <c r="E8" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
@@ -837,8 +829,8 @@
         <v>14</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="8" t="s">
-        <v>56</v>
+      <c r="E10" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
@@ -855,7 +847,7 @@
       <c r="D11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="2" t="s">
         <v>40</v>
       </c>
@@ -871,8 +863,8 @@
         <v>15</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="11" t="s">
-        <v>57</v>
+      <c r="E12" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
@@ -889,11 +881,11 @@
       <c r="D13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="13"/>
+      <c r="F13" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="17"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -905,11 +897,11 @@
         <v>16</v>
       </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
+      <c r="E14" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17" t="s">
         <v>43</v>
       </c>
     </row>
@@ -925,10 +917,10 @@
         <v>31</v>
       </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
@@ -940,8 +932,8 @@
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="18"/>
+      <c r="G16" s="18" t="s">
         <v>45</v>
       </c>
     </row>
@@ -955,8 +947,8 @@
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
@@ -968,8 +960,8 @@
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
@@ -981,8 +973,8 @@
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
@@ -993,11 +985,11 @@
         <v>17</v>
       </c>
       <c r="D20" s="9"/>
-      <c r="E20" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="E20" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
@@ -1009,10 +1001,10 @@
         <v>32</v>
       </c>
       <c r="E21" s="9"/>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
@@ -1026,8 +1018,8 @@
       <c r="E22" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5" t="s">
+      <c r="F22" s="18"/>
+      <c r="G22" s="18" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1041,10 +1033,10 @@
         <v>31</v>
       </c>
       <c r="E23" s="9"/>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
@@ -1060,8 +1052,8 @@
       <c r="E24" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6" t="s">
+      <c r="F24" s="19"/>
+      <c r="G24" s="19" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1075,10 +1067,10 @@
         <v>31</v>
       </c>
       <c r="E25" s="10"/>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="6"/>
+      <c r="G25" s="19"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
@@ -1089,11 +1081,11 @@
         <v>20</v>
       </c>
       <c r="D26" s="10"/>
-      <c r="E26" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6" t="s">
+      <c r="E26" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1107,10 +1099,10 @@
         <v>33</v>
       </c>
       <c r="E27" s="10"/>
-      <c r="F27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="6"/>
+      <c r="F27" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="19"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
@@ -1124,9 +1116,9 @@
       <c r="E28" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6" t="s">
-        <v>61</v>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
final changes for start of semester
</commit_message>
<xml_diff>
--- a/teaching/expdes/master-plan.xlsx
+++ b/teaching/expdes/master-plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="44940" yWindow="460" windowWidth="24320" windowHeight="20320" tabRatio="500"/>
+    <workbookView xWindow="55180" yWindow="860" windowWidth="24320" windowHeight="20320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>January</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>HW6 finish - plant</t>
+  </si>
+  <si>
+    <t>HW6</t>
+  </si>
+  <si>
+    <t>HW7 finish - book-probs</t>
+  </si>
+  <si>
+    <t>HW7</t>
   </si>
 </sst>
 </file>
@@ -641,7 +650,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -917,8 +926,10 @@
       <c r="F14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -929,12 +940,14 @@
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="9" t="s">
-        <v>29</v>
+      <c r="E15" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="F15" s="9"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="G15" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
@@ -949,8 +962,10 @@
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>

</xml_diff>